<commit_message>
Joined socio and life expectancy dataframes.
</commit_message>
<xml_diff>
--- a/Sean/Trials/Trial 36.xlsx
+++ b/Sean/Trials/Trial 36.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="18">
   <si>
     <t>Epoch Cost</t>
   </si>
@@ -425,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3978,6 +3978,56 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="72" spans="1:16">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>5.163888454437256</v>
+      </c>
+      <c r="C72">
+        <v>0.2256377190351486</v>
+      </c>
+      <c r="D72">
+        <v>0.2287076711654663</v>
+      </c>
+      <c r="E72">
+        <v>48.17729687690735</v>
+      </c>
+      <c r="F72">
+        <v>0.01</v>
+      </c>
+      <c r="G72">
+        <v>0.01</v>
+      </c>
+      <c r="H72">
+        <v>0.98</v>
+      </c>
+      <c r="I72">
+        <v>0.001</v>
+      </c>
+      <c r="J72">
+        <v>10000</v>
+      </c>
+      <c r="K72" t="s">
+        <v>15</v>
+      </c>
+      <c r="L72">
+        <v>100</v>
+      </c>
+      <c r="M72">
+        <v>14</v>
+      </c>
+      <c r="N72" t="s">
+        <v>16</v>
+      </c>
+      <c r="O72" t="s">
+        <v>17</v>
+      </c>
+      <c r="P72">
+        <v>0.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>